<commit_message>
update food insecure fraction according to LiST
</commit_message>
<xml_diff>
--- a/Input_LiST_Bangladesh.xlsx
+++ b/Input_LiST_Bangladesh.xlsx
@@ -28,10 +28,6 @@
     <sheet state="visible" name="Interventions affected fraction" sheetId="23" r:id="rId25"/>
     <sheet state="visible" name="Interventions mortality eff" sheetId="24" r:id="rId26"/>
     <sheet state="visible" name="Interventions incidence eff" sheetId="25" r:id="rId27"/>
-    <sheet state="visible" name="RR birth by type" sheetId="26" r:id="rId28"/>
-    <sheet state="visible" name="birth distribution" sheetId="27" r:id="rId29"/>
-    <sheet state="visible" name="time between births" sheetId="28" r:id="rId30"/>
-    <sheet state="visible" name="RR birth by time" sheetId="29" r:id="rId31"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -71,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="78">
   <si>
     <t>indicators</t>
   </si>
@@ -305,36 +301,6 @@
   </si>
   <si>
     <t>Interventions</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>&lt;18 years</t>
-  </si>
-  <si>
-    <t>18-34 years</t>
-  </si>
-  <si>
-    <t>35-49 years</t>
-  </si>
-  <si>
-    <t>first</t>
-  </si>
-  <si>
-    <t>second or third</t>
-  </si>
-  <si>
-    <t>greater than third</t>
-  </si>
-  <si>
-    <t>&lt;18 months</t>
-  </si>
-  <si>
-    <t>18-23 months</t>
-  </si>
-  <si>
-    <t>&lt;24 months</t>
   </si>
 </sst>
 </file>
@@ -397,7 +363,6 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -414,6 +379,7 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment/>
     </xf>
@@ -522,22 +488,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing26.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing27.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing28.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing29.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
 <file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
@@ -612,8 +562,8 @@
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
-        <v>0.3</v>
+      <c r="B5" s="2">
+        <v>0.44</v>
       </c>
     </row>
     <row r="6">
@@ -639,7 +589,7 @@
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="10" t="s">
         <v>53</v>
       </c>
       <c r="C1" t="s">
@@ -653,152 +603,152 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="10">
         <v>1.0</v>
       </c>
       <c r="C2">
         <v>1.0</v>
       </c>
-      <c r="D2" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="D2" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="10">
         <v>1.0</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="10">
         <v>1.0</v>
       </c>
       <c r="C3">
         <v>2.07</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="10">
         <v>8.02</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="10">
         <v>11.54</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="10">
         <v>1.0</v>
       </c>
       <c r="C4">
         <v>2.07</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="10">
         <v>8.02</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="10">
         <v>11.54</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="10">
         <v>1.0</v>
       </c>
       <c r="C5">
         <v>2.07</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="10">
         <v>8.02</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="10">
         <v>11.54</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="10">
         <v>1.0</v>
       </c>
       <c r="C6">
         <v>1.0</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="10">
         <v>999.99</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="10">
         <v>999.99</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="10">
         <v>1.0</v>
       </c>
       <c r="C7">
         <v>1.0</v>
       </c>
-      <c r="D7" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="D7" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="10">
         <v>1.0</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="10">
         <v>1.0</v>
       </c>
       <c r="C8">
         <v>1.0</v>
       </c>
-      <c r="D8" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="D8" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="10">
         <v>1.0</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="10">
         <v>1.0</v>
       </c>
       <c r="C9">
         <v>1.0</v>
       </c>
-      <c r="D9" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="D9" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="10">
         <v>1.0</v>
       </c>
       <c r="F9" s="2"/>
@@ -1461,13 +1411,13 @@
       <c r="A2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>5.16</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>5.16</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>1.82</v>
       </c>
       <c r="E2" s="14">
@@ -1526,16 +1476,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -1573,122 +1523,131 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
+        <v>2016.0</v>
+      </c>
+      <c r="B2" s="6" t="str">
+        <f>demographics!$B$3</f>
+        <v>3,030,000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5">
         <v>2017.0</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B3" s="6">
         <v>3010000.0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="6">
+    <row r="4">
+      <c r="A4" s="5">
         <v>2018.0</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B4" s="6">
         <v>2980000.0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="6">
+    <row r="5">
+      <c r="A5" s="5">
         <v>2019.0</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B5" s="6">
         <v>2960000.0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="6">
+    <row r="6">
+      <c r="A6" s="5">
         <v>2020.0</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B6" s="6">
         <v>2930000.0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="6">
+    <row r="7">
+      <c r="A7" s="5">
         <v>2021.0</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B7" s="6">
         <v>2900000.0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="6">
+    <row r="8">
+      <c r="A8" s="5">
         <v>2022.0</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B8" s="6">
         <v>2870000.0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="6">
+    <row r="9">
+      <c r="A9" s="5">
         <v>2023.0</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B9" s="6">
         <v>2840000.0</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="6">
+    <row r="10">
+      <c r="A10" s="5">
         <v>2024.0</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B10" s="6">
         <v>2810000.0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="6">
+    <row r="11">
+      <c r="A11" s="5">
         <v>2025.0</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B11" s="6">
         <v>2780000.0</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="6">
+    <row r="12">
+      <c r="A12" s="5">
         <v>2026.0</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B12" s="6">
         <v>2740000.0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="6">
+    <row r="13">
+      <c r="A13" s="5">
         <v>2027.0</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B13" s="6">
         <v>2710000.0</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="6">
+    <row r="14">
+      <c r="A14" s="5">
         <v>2028.0</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B14" s="6">
         <v>2670000.0</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="6">
+    <row r="15">
+      <c r="A15" s="5">
         <v>2029.0</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B15" s="6">
         <v>2640000.0</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="6">
+    <row r="16">
+      <c r="A16" s="5">
         <v>2030.0</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B16" s="6">
         <v>2600000.0</v>
       </c>
     </row>
@@ -1827,7 +1786,7 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="10" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="2">
@@ -1989,22 +1948,22 @@
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F2" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="G2" s="6">
+      <c r="B2" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="G2" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -2012,22 +1971,22 @@
       <c r="A3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="6">
+      <c r="B3" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -2035,22 +1994,22 @@
       <c r="A4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="G4" s="6">
+      <c r="B4" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -2058,26 +2017,26 @@
       <c r="A5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="C5" s="6" t="str">
+      <c r="B5" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C5" s="5" t="str">
         <f>demographics!$B$5</f>
-        <v>0.3</v>
-      </c>
-      <c r="D5" s="6" t="str">
+        <v>0.44</v>
+      </c>
+      <c r="D5" s="5" t="str">
         <f>demographics!$B$5</f>
-        <v>0.3</v>
-      </c>
-      <c r="E5" s="6" t="str">
+        <v>0.44</v>
+      </c>
+      <c r="E5" s="5" t="str">
         <f>demographics!$B$5</f>
-        <v>0.3</v>
-      </c>
-      <c r="F5" s="6" t="str">
+        <v>0.44</v>
+      </c>
+      <c r="F5" s="5" t="str">
         <f>demographics!$B$5</f>
-        <v>0.3</v>
-      </c>
-      <c r="G5" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="G5" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -2085,22 +2044,22 @@
       <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="G6" s="6">
+      <c r="B6" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -2108,45 +2067,45 @@
       <c r="A7" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="G7" s="6">
+      <c r="B7" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="G7" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="F8" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="G8" s="6">
+      <c r="B8" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="5">
         <v>1.0</v>
       </c>
     </row>
@@ -2308,15 +2267,15 @@
       </c>
       <c r="C3" s="18" t="str">
         <f>demographics!$B$5</f>
-        <v>0.30</v>
+        <v>0.44</v>
       </c>
       <c r="D3" s="18" t="str">
         <f>demographics!$B$5</f>
-        <v>0.30</v>
+        <v>0.44</v>
       </c>
       <c r="E3" s="18" t="str">
         <f>demographics!$B$5</f>
-        <v>0.30</v>
+        <v>0.44</v>
       </c>
       <c r="F3" s="18">
         <v>0.0</v>
@@ -2662,6 +2621,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="23.0"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
@@ -2793,361 +2755,6 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3.14</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.73</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.6</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1.52</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.52</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.0543</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.1711</v>
-      </c>
-      <c r="D2" s="2">
-        <v>3.0E-4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.009</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.3607</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.0085</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.2908</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.1048</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2">
-        <v>0.2258</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.0705</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.134</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.5698</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3.03</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.77</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.49</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.41</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1.18</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.0</v>
-      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3173,13 +2780,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8">
+      <c r="A2" s="7">
         <v>23.3</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>30.7</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>37.6</v>
       </c>
     </row>
@@ -3220,7 +2827,7 @@
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>0.007</v>
       </c>
       <c r="C2" s="2">
@@ -3240,7 +2847,7 @@
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>0.199</v>
       </c>
       <c r="C3" s="2">
@@ -3260,7 +2867,7 @@
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>0.059</v>
       </c>
       <c r="C4" s="2">
@@ -3280,7 +2887,7 @@
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>0.229</v>
       </c>
       <c r="C5" s="2">
@@ -3300,7 +2907,7 @@
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>0.297</v>
       </c>
       <c r="C6" s="2">
@@ -3320,7 +2927,7 @@
       <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>0.006</v>
       </c>
       <c r="C7" s="2">
@@ -3340,7 +2947,7 @@
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>0.127</v>
       </c>
       <c r="C8" s="2">
@@ -3360,7 +2967,7 @@
       <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>0.076</v>
       </c>
       <c r="C9" s="2">
@@ -3380,19 +2987,19 @@
       <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="C10" s="9">
+      <c r="B10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C10" s="8">
         <v>0.1481</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>0.1481</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>0.1481</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>0.1481</v>
       </c>
     </row>
@@ -3400,19 +3007,19 @@
       <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="C11" s="9">
+      <c r="B11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C11" s="8">
         <v>0.2883</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>0.2883</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>0.2883</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>0.2883</v>
       </c>
     </row>
@@ -3420,19 +3027,19 @@
       <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="C12" s="9">
+      <c r="B12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="C12" s="8">
         <v>0.041</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>0.041</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>0.041</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>0.041</v>
       </c>
     </row>
@@ -3443,16 +3050,16 @@
       <c r="B13" s="2">
         <v>0.0</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>0.05</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>0.05</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>0.05</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>0.05</v>
       </c>
     </row>
@@ -3463,16 +3070,16 @@
       <c r="B14" s="2">
         <v>0.0</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>0.006</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>0.006</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>0.006</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>0.006</v>
       </c>
     </row>
@@ -3483,16 +3090,16 @@
       <c r="B15" s="2">
         <v>0.0</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>0.01</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>0.01</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>0.01</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>0.01</v>
       </c>
     </row>
@@ -3503,16 +3110,16 @@
       <c r="B16" s="2">
         <v>0.0</v>
       </c>
-      <c r="C16" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="E16" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="F16" s="9">
+      <c r="C16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F16" s="8">
         <v>0.0</v>
       </c>
     </row>
@@ -3523,16 +3130,16 @@
       <c r="B17" s="2">
         <v>0.0</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="8">
         <v>0.1451</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <v>0.1451</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="8">
         <v>0.1451</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <v>0.1451</v>
       </c>
     </row>
@@ -3543,16 +3150,16 @@
       <c r="B18" s="2">
         <v>0.0</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>0.3115</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <v>0.3115</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>0.3115</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="8">
         <v>0.3115</v>
       </c>
     </row>
@@ -3598,19 +3205,19 @@
       <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>60.67</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>60.67</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>47.206</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>22.921</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="9">
         <v>23.661</v>
       </c>
     </row>
@@ -3618,19 +3225,19 @@
       <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>21.637</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>21.637</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>30.252</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>27.735</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <v>31.069</v>
       </c>
     </row>
@@ -3638,19 +3245,19 @@
       <c r="B4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>13.337</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>13.337</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>14.065</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>30.803</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <v>28.443</v>
       </c>
     </row>
@@ -3658,19 +3265,19 @@
       <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>4.356</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>4.356</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>8.477</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>18.541</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>16.827</v>
       </c>
     </row>
@@ -3681,19 +3288,19 @@
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>60.66</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>60.66</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>47.21</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>22.93</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>23.66</v>
       </c>
     </row>
@@ -3701,19 +3308,19 @@
       <c r="B7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>21.64</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>21.64</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>30.25</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>27.73</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>31.07</v>
       </c>
     </row>
@@ -3721,19 +3328,19 @@
       <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>13.34</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>13.34</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>14.06</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <v>30.8</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <v>28.44</v>
       </c>
     </row>
@@ -3741,19 +3348,19 @@
       <c r="B9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>4.36</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>4.36</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>8.48</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>18.54</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>16.83</v>
       </c>
     </row>
@@ -3764,19 +3371,19 @@
       <c r="B10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>87.6</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>61.0</v>
       </c>
-      <c r="E10" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="F10" s="10">
-        <v>0.0</v>
-      </c>
-      <c r="G10" s="4">
+      <c r="E10" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="G10" s="10">
         <v>0.0</v>
       </c>
     </row>
@@ -3784,19 +3391,19 @@
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>3.5</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>13.9</v>
       </c>
-      <c r="E11" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="G11" s="4">
+      <c r="E11" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="10">
         <v>0.0</v>
       </c>
     </row>
@@ -3804,19 +3411,19 @@
       <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>8.9</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>24.2</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>96.4</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="9">
         <v>93.1</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="10">
         <v>0.0</v>
       </c>
     </row>
@@ -3824,19 +3431,19 @@
       <c r="B13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E13" s="10">
+      <c r="C13" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="9">
         <v>3.6</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="9">
         <v>6.9</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="10">
         <v>100.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
LiST specific food-security; fix ORstuntingProgression and target pop for complementary feeding
</commit_message>
<xml_diff>
--- a/Input_LiST_Bangladesh.xlsx
+++ b/Input_LiST_Bangladesh.xlsx
@@ -889,7 +889,7 @@
         <v>11.2</v>
       </c>
       <c r="B2" s="2">
-        <v>26.9</v>
+        <v>268.7</v>
       </c>
       <c r="C2" s="2">
         <v>67.3</v>
@@ -1998,7 +1998,7 @@
         <v>0.0</v>
       </c>
       <c r="C4" s="5">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D4" s="5">
         <v>1.0</v>
@@ -2020,9 +2020,8 @@
       <c r="B5" s="5">
         <v>0.0</v>
       </c>
-      <c r="C5" s="5" t="str">
-        <f>demographics!$B$5</f>
-        <v>0.44</v>
+      <c r="C5" s="5">
+        <v>0.0</v>
       </c>
       <c r="D5" s="5" t="str">
         <f>demographics!$B$5</f>

</xml_diff>